<commit_message>
Usunieta zawartość z pliku notes_data.xlsx
</commit_message>
<xml_diff>
--- a/notes_data.xlsx
+++ b/notes_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="127">
   <si>
     <t xml:space="preserve">Przepisać wartość z G2</t>
   </si>
@@ -35,130 +35,61 @@
     <t xml:space="preserve">pracownik1</t>
   </si>
   <si>
-    <t xml:space="preserve">Andrzejak Adrianna</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik2</t>
   </si>
   <si>
-    <t xml:space="preserve">Atłas Agata</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik3</t>
   </si>
   <si>
-    <t xml:space="preserve">Jacyno Nicoletta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jankowska Ernestyna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janowska Monika</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kazimierczak Klaudia</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik7</t>
   </si>
   <si>
-    <t xml:space="preserve">Kistowska Klaudia</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik8</t>
   </si>
   <si>
-    <t xml:space="preserve">Krawiec Paulina</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik9</t>
   </si>
   <si>
-    <t xml:space="preserve">Ługowska Ina</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik10</t>
   </si>
   <si>
-    <t xml:space="preserve">Maciejewska Monika</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik11</t>
   </si>
   <si>
-    <t xml:space="preserve">Manicka Dagmara</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik12</t>
   </si>
   <si>
-    <t xml:space="preserve">Myszka Aleksandra</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik13</t>
   </si>
   <si>
-    <t xml:space="preserve">Nowacka Martyna</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik14</t>
   </si>
   <si>
-    <t xml:space="preserve">Nowak Wiktoria</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik15</t>
   </si>
   <si>
-    <t xml:space="preserve">Olkuśnik Magdalena</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik16</t>
   </si>
   <si>
-    <t xml:space="preserve">Rutkowska Julita</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik17</t>
   </si>
   <si>
-    <t xml:space="preserve">Stefanowicz Roksana</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik18</t>
   </si>
   <si>
-    <t xml:space="preserve">Stephan Klaudia</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik19</t>
   </si>
   <si>
-    <t xml:space="preserve">Swyszcz Małgorzata</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik20</t>
   </si>
   <si>
-    <t xml:space="preserve">Szaroleta Klaudia</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik21</t>
   </si>
   <si>
-    <t xml:space="preserve">Szymoniak Karolina</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik22</t>
   </si>
   <si>
-    <t xml:space="preserve">Śleziona Olga</t>
-  </si>
-  <si>
     <t xml:space="preserve">pracownik23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zydorczak Barbara</t>
   </si>
   <si>
     <t xml:space="preserve">pracownik24</t>
@@ -586,10 +517,10 @@
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.24"/>
   </cols>
@@ -610,7 +541,7 @@
       <c r="C2" s="1"/>
       <c r="G2" s="0" t="n">
         <f aca="false">SUM(D4:D87)</f>
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>23</v>
@@ -630,16 +561,14 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="0" t="n">
         <f aca="false">IF(2=E4,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">TYPE(C4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,18 +576,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(2=E5,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">TYPE(C5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -667,38 +594,34 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(2=E6,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">TYPE(C6)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="0" t="n">
         <f aca="false">IF(2=E7,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">TYPE(C7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -707,18 +630,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="0" t="n">
         <f aca="false">IF(2=E8,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">TYPE(C8)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -727,18 +648,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="0" t="n">
         <f aca="false">IF(2=E9,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">TYPE(C9)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -747,18 +666,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="0" t="n">
         <f aca="false">IF(2=E10,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">TYPE(C10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -767,18 +684,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(2=E11,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">TYPE(C11)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="3"/>
     </row>
@@ -787,18 +702,16 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(2=E12,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">TYPE(C12)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="3"/>
     </row>
@@ -807,18 +720,16 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="0" t="n">
         <f aca="false">IF(2=E13,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">TYPE(C13)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="3"/>
     </row>
@@ -827,18 +738,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(2=E14,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">TYPE(C14)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -847,18 +756,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="0" t="n">
         <f aca="false">IF(2=E15,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">TYPE(C15)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3"/>
     </row>
@@ -867,18 +774,16 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="0" t="n">
         <f aca="false">IF(2=E16,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">TYPE(C16)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -887,18 +792,16 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="0" t="n">
         <f aca="false">IF(2=E17,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">TYPE(C17)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -907,18 +810,16 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="0" t="n">
         <f aca="false">IF(2=E18,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">TYPE(C18)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -927,18 +828,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="0" t="n">
         <f aca="false">IF(2=E19,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">TYPE(C19)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3"/>
     </row>
@@ -947,18 +846,16 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="0" t="n">
         <f aca="false">IF(2=E20,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="0" t="n">
         <f aca="false">TYPE(C20)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="3"/>
     </row>
@@ -967,18 +864,16 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C21" s="2"/>
       <c r="D21" s="0" t="n">
         <f aca="false">IF(2=E21,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="0" t="n">
         <f aca="false">TYPE(C21)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3"/>
     </row>
@@ -987,18 +882,16 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C22" s="2"/>
       <c r="D22" s="0" t="n">
         <f aca="false">IF(2=E22,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">TYPE(C22)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="3"/>
     </row>
@@ -1007,18 +900,16 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C23" s="2"/>
       <c r="D23" s="0" t="n">
         <f aca="false">IF(2=E23,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="0" t="n">
         <f aca="false">TYPE(C23)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3"/>
     </row>
@@ -1027,18 +918,16 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C24" s="2"/>
       <c r="D24" s="0" t="n">
         <f aca="false">IF(2=E24,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="0" t="n">
         <f aca="false">TYPE(C24)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -1047,18 +936,16 @@
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="0" t="n">
         <f aca="false">IF(2=E25,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="0" t="n">
         <f aca="false">TYPE(C25)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3"/>
     </row>
@@ -1067,18 +954,16 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="0" t="n">
         <f aca="false">IF(2=E26,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="0" t="n">
         <f aca="false">TYPE(C26)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" s="3"/>
     </row>
@@ -1087,7 +972,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="0" t="n">
@@ -1105,7 +990,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="0" t="n">
@@ -1123,7 +1008,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="0" t="n">
@@ -1141,7 +1026,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="0" t="n">
@@ -1159,7 +1044,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="0" t="n">
@@ -1177,7 +1062,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="0" t="n">
@@ -1195,7 +1080,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="0" t="n">
@@ -1213,7 +1098,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="0" t="n">
@@ -1231,7 +1116,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="0" t="n">
@@ -1249,7 +1134,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="0" t="n">
@@ -1267,7 +1152,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="0" t="n">
@@ -1285,7 +1170,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D38" s="0" t="n">
         <f aca="false">IF(2=E38,1,0)</f>
@@ -1302,7 +1187,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D39" s="0" t="n">
         <f aca="false">IF(2=E39,1,0)</f>
@@ -1318,7 +1203,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D40" s="0" t="n">
         <f aca="false">IF(2=E40,1,0)</f>
@@ -1334,7 +1219,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D41" s="0" t="n">
         <f aca="false">IF(2=E41,1,0)</f>
@@ -1350,7 +1235,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D42" s="0" t="n">
         <f aca="false">IF(2=E42,1,0)</f>
@@ -1366,7 +1251,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D43" s="0" t="n">
         <f aca="false">IF(2=E43,1,0)</f>
@@ -1382,7 +1267,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D44" s="0" t="n">
         <f aca="false">IF(2=E44,1,0)</f>
@@ -1398,7 +1283,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D45" s="0" t="n">
         <f aca="false">IF(2=E45,1,0)</f>
@@ -1414,7 +1299,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D46" s="0" t="n">
         <f aca="false">IF(2=E46,1,0)</f>
@@ -1430,7 +1315,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="D47" s="0" t="n">
         <f aca="false">IF(2=E47,1,0)</f>
@@ -1446,7 +1331,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D48" s="0" t="n">
         <f aca="false">IF(2=E48,1,0)</f>
@@ -1462,7 +1347,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D49" s="0" t="n">
         <f aca="false">IF(2=E49,1,0)</f>
@@ -1478,7 +1363,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D50" s="0" t="n">
         <f aca="false">IF(2=E50,1,0)</f>
@@ -1494,7 +1379,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D51" s="0" t="n">
         <f aca="false">IF(2=E51,1,0)</f>
@@ -1510,7 +1395,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D52" s="0" t="n">
         <f aca="false">IF(2=E52,1,0)</f>
@@ -1526,7 +1411,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D53" s="0" t="n">
         <f aca="false">IF(2=E53,1,0)</f>
@@ -1542,7 +1427,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D54" s="0" t="n">
         <f aca="false">IF(2=E54,1,0)</f>
@@ -1558,7 +1443,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D55" s="0" t="n">
         <f aca="false">IF(2=E55,1,0)</f>
@@ -1574,7 +1459,7 @@
         <v>53</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D56" s="0" t="n">
         <f aca="false">IF(2=E56,1,0)</f>
@@ -1590,7 +1475,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D57" s="0" t="n">
         <f aca="false">IF(2=E57,1,0)</f>
@@ -1606,7 +1491,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D58" s="0" t="n">
         <f aca="false">IF(2=E58,1,0)</f>
@@ -1622,7 +1507,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D59" s="0" t="n">
         <f aca="false">IF(2=E59,1,0)</f>
@@ -1638,7 +1523,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(2=E60,1,0)</f>
@@ -1654,7 +1539,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="0" t="n">
@@ -1671,7 +1556,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D62" s="0" t="n">
         <f aca="false">IF(2=E62,1,0)</f>
@@ -1687,7 +1572,7 @@
         <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D63" s="0" t="n">
         <f aca="false">IF(2=E63,1,0)</f>
@@ -1703,7 +1588,7 @@
         <v>61</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="D64" s="0" t="n">
         <f aca="false">IF(2=E64,1,0)</f>
@@ -1719,7 +1604,7 @@
         <v>62</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D65" s="0" t="n">
         <f aca="false">IF(2=E65,1,0)</f>
@@ -1735,7 +1620,7 @@
         <v>63</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="D66" s="0" t="n">
         <f aca="false">IF(2=E66,1,0)</f>
@@ -1751,7 +1636,7 @@
         <v>64</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D67" s="0" t="n">
         <f aca="false">IF(2=E67,1,0)</f>
@@ -1767,7 +1652,7 @@
         <v>65</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D68" s="0" t="n">
         <f aca="false">IF(2=E68,1,0)</f>
@@ -1783,7 +1668,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="D69" s="0" t="n">
         <f aca="false">IF(2=E69,1,0)</f>
@@ -1799,7 +1684,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="D70" s="0" t="n">
         <f aca="false">IF(2=E70,1,0)</f>
@@ -1815,7 +1700,7 @@
         <v>68</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(2=E71,1,0)</f>
@@ -1831,7 +1716,7 @@
         <v>69</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="D72" s="0" t="n">
         <f aca="false">IF(2=E72,1,0)</f>
@@ -1847,7 +1732,7 @@
         <v>70</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D73" s="0" t="n">
         <f aca="false">IF(2=E73,1,0)</f>
@@ -1863,7 +1748,7 @@
         <v>71</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="D74" s="0" t="n">
         <f aca="false">IF(2=E74,1,0)</f>
@@ -1879,7 +1764,7 @@
         <v>72</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D75" s="0" t="n">
         <f aca="false">IF(2=E75,1,0)</f>
@@ -1895,7 +1780,7 @@
         <v>73</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D76" s="0" t="n">
         <f aca="false">IF(2=E76,1,0)</f>
@@ -1911,7 +1796,7 @@
         <v>74</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">IF(2=E77,1,0)</f>
@@ -1927,7 +1812,7 @@
         <v>75</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="D78" s="0" t="n">
         <f aca="false">IF(2=E78,1,0)</f>
@@ -1943,7 +1828,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="D79" s="0" t="n">
         <f aca="false">IF(2=E79,1,0)</f>
@@ -1959,7 +1844,7 @@
         <v>77</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="D80" s="0" t="n">
         <f aca="false">IF(2=E80,1,0)</f>
@@ -1975,7 +1860,7 @@
         <v>78</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="D81" s="0" t="n">
         <f aca="false">IF(2=E81,1,0)</f>
@@ -1991,7 +1876,7 @@
         <v>79</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D82" s="0" t="n">
         <f aca="false">IF(2=E82,1,0)</f>
@@ -2007,7 +1892,7 @@
         <v>80</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="D83" s="0" t="n">
         <f aca="false">IF(2=E83,1,0)</f>
@@ -2023,7 +1908,7 @@
         <v>81</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="D84" s="0" t="n">
         <f aca="false">IF(2=E84,1,0)</f>
@@ -2039,7 +1924,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="D85" s="0" t="n">
         <f aca="false">IF(2=E85,1,0)</f>
@@ -2055,7 +1940,7 @@
         <v>83</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="D86" s="0" t="n">
         <f aca="false">IF(2=E86,1,0)</f>
@@ -2071,7 +1956,7 @@
         <v>84</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="D87" s="0" t="n">
         <f aca="false">IF(2=E87,1,0)</f>
@@ -2087,7 +1972,7 @@
         <v>85</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="D88" s="0" t="n">
         <f aca="false">IF(2=E88,1,0)</f>
@@ -2103,7 +1988,7 @@
         <v>86</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="D89" s="0" t="n">
         <f aca="false">IF(2=E89,1,0)</f>
@@ -2119,7 +2004,7 @@
         <v>87</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="D90" s="0" t="n">
         <f aca="false">IF(2=E90,1,0)</f>
@@ -2135,7 +2020,7 @@
         <v>88</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="D91" s="0" t="n">
         <f aca="false">IF(2=E91,1,0)</f>
@@ -2151,7 +2036,7 @@
         <v>89</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D92" s="0" t="n">
         <f aca="false">IF(2=E92,1,0)</f>
@@ -2167,7 +2052,7 @@
         <v>90</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D93" s="0" t="n">
         <f aca="false">IF(2=E93,1,0)</f>
@@ -2183,7 +2068,7 @@
         <v>91</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D94" s="0" t="n">
         <f aca="false">IF(2=E94,1,0)</f>
@@ -2199,7 +2084,7 @@
         <v>92</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="D95" s="0" t="n">
         <f aca="false">IF(2=E95,1,0)</f>
@@ -2215,7 +2100,7 @@
         <v>93</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="D96" s="0" t="n">
         <f aca="false">IF(2=E96,1,0)</f>
@@ -2248,179 +2133,179 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>